<commit_message>
Begin processing for 2022-23
</commit_message>
<xml_diff>
--- a/data/rid_resa_nve_discharge_stations.xlsx
+++ b/data/rid_resa_nve_discharge_stations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Oeyvind_K\Elveovervakingsprogrammet\Python\rid\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D17368-FE5B-4D45-B4CE-D7D45CD9F30E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FE04D0-73B2-472F-84A0-DCB73EEA5139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{CBC9E924-6FFF-45C6-A5D0-1CBEBADDAA61}"/>
+    <workbookView xWindow="31680" yWindow="2355" windowWidth="21600" windowHeight="12600" xr2:uid="{CBC9E924-6FFF-45C6-A5D0-1CBEBADDAA61}"/>
   </bookViews>
   <sheets>
     <sheet name="observed_stns" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>62.5.0</t>
   </si>
   <si>
-    <t>6.78.0</t>
-  </si>
-  <si>
     <t>Not available via API</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Used to be 151.5.0, but this is not available via API. 151.28.0 seems identical</t>
+  </si>
+  <si>
+    <t>Used to be 6.78.0 (dis_stn 626), but switched to modelled series due to difficulties obtaining data</t>
   </si>
 </sst>
 </file>
@@ -492,19 +492,19 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="87.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="87.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -521,7 +521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>29612</v>
       </c>
@@ -535,10 +535,10 @@
         <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>29613</v>
       </c>
@@ -555,7 +555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>29614</v>
       </c>
@@ -569,10 +569,10 @@
         <v>487</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>29615</v>
       </c>
@@ -586,7 +586,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>29617</v>
       </c>
@@ -600,7 +600,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>29778</v>
       </c>
@@ -614,7 +614,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>29779</v>
       </c>
@@ -628,7 +628,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>29782</v>
       </c>
@@ -636,16 +636,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9">
         <v>351</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>29783</v>
       </c>
@@ -659,7 +659,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>29821</v>
       </c>
@@ -673,18 +673,15 @@
         <v>546</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>36225</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12">
-        <v>626</v>
+      <c r="E12" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial processing of 2023 data
</commit_message>
<xml_diff>
--- a/data/rid_resa_nve_discharge_stations.xlsx
+++ b/data/rid_resa_nve_discharge_stations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FE04D0-73B2-472F-84A0-DCB73EEA5139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C652307-D250-4C15-9DC4-032022EE235A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31680" yWindow="2355" windowWidth="21600" windowHeight="12600" xr2:uid="{CBC9E924-6FFF-45C6-A5D0-1CBEBADDAA61}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{CBC9E924-6FFF-45C6-A5D0-1CBEBADDAA61}"/>
   </bookViews>
   <sheets>
     <sheet name="observed_stns" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>BUSEDRA</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>62.5.0</t>
-  </si>
-  <si>
-    <t>Not available via API</t>
   </si>
   <si>
     <t>151.28.0</t>
@@ -193,9 +190,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -233,7 +230,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -339,7 +336,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -481,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -492,7 +489,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,9 +531,6 @@
       <c r="D2">
         <v>57</v>
       </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -568,9 +562,6 @@
       <c r="D4">
         <v>487</v>
       </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -636,13 +627,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9">
         <v>351</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -681,7 +672,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>